<commit_message>
Update the testcase Rincian Supplier. Add testcase Edit Supplier, TambahAlamatSupplier, EditAlamatSupplier, HapusAlamatSupplier
</commit_message>
<xml_diff>
--- a/Excel/SupplierDataExcel.xlsx
+++ b/Excel/SupplierDataExcel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>namasupplier</t>
   </si>
@@ -65,9 +65,6 @@
     <t>alamatlengkap</t>
   </si>
   <si>
-    <t>alamatfaktur</t>
-  </si>
-  <si>
     <t>namapj</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
   </si>
   <si>
     <t>Jl. Alamat Lengkap 1</t>
-  </si>
-  <si>
-    <t>Gang Alamat Faktur</t>
   </si>
   <si>
     <t>PJ Tumirah</t>
@@ -1290,10 +1284,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="M1" sqref="M$1:M$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -1307,10 +1301,9 @@
     <col min="8" max="8" width="18.6363636363636" customWidth="1"/>
     <col min="10" max="11" width="11.2727272727273" customWidth="1"/>
     <col min="12" max="12" width="19.3636363636364" customWidth="1"/>
-    <col min="13" max="13" width="15.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:16">
+    <row r="1" s="1" customFormat="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1356,64 +1349,58 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:15">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" s="2" customFormat="1" spans="1:16">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="5" tooltip="mailto:tumirah@gmail.com"/>
-    <hyperlink ref="P2" r:id="rId2" display="pjtumirah@mail.com" tooltip="mailto:pjtumirah@mail.com"/>
+    <hyperlink ref="O2" r:id="rId2" display="pjtumirah@mail.com" tooltip="mailto:pjtumirah@mail.com"/>
     <hyperlink ref="H2" r:id="rId3" display="tumirah@mail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>